<commit_message>
modification etat eleve hyper planning
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/ETUDIANTS.xlsx
+++ b/src/main/resources/templates/ETUDIANTS.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Projets\kranja-pigier-backend\src\main\resources\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,68 +24,52 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">LISTE DES ETUDIANTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>LISTE DES ETUDIANTS</t>
+  </si>
+  <si>
+    <t>Nom</t>
   </si>
   <si>
     <t xml:space="preserve">Prénom </t>
   </si>
   <si>
-    <t xml:space="preserve">Né(e) le</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sexe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Promotions</t>
+    <t>Né(e) le</t>
+  </si>
+  <si>
+    <t>Sexe</t>
+  </si>
+  <si>
+    <t>Promotions</t>
   </si>
   <si>
     <t xml:space="preserve">E-mail institutionnel </t>
   </si>
   <si>
-    <t xml:space="preserve">Destinataire des courriers</t>
-  </si>
-  <si>
     <t xml:space="preserve">Numéro étudiants </t>
   </si>
   <si>
-    <t xml:space="preserve">Numéro parents</t>
+    <t>Numéro parents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matricule </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lieu de naissance </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,7 +81,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -101,101 +89,80 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -227,7 +194,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -251,7 +218,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -311,79 +278,81 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="29.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="G3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="H3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="I3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="J3" t="s">
         <v>8</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>